<commit_message>
Completed working version for phs000463
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC02_CCDI_phs000463_DiagAnatSite-C42.0Blood_FirsEvent-Death.xlsx
+++ b/InputFiles/CCDI/TC02_CCDI_phs000463_DiagAnatSite-C42.0Blood_FirsEvent-Death.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5196CF-FA4B-4887-B981-CF4F75B36B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BBD27C-442B-284A-BE02-F840DB4F55C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-5840" yWindow="-25780" windowWidth="37540" windowHeight="20920" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,47 +63,6 @@
   </si>
   <si>
     <t>StudiesTab</t>
-  </si>
-  <si>
-    <t>with file_data as (
-select file_name, data_category, file_type, file_size, file_access, file_description,"study.id" studyid, "participant.id" as participantid from df_clinical_measure_file )
-SELECT fd.file_name AS "File Name",
-    fd.data_category AS "Data Category",
-    COALESCE(fd.file_description, '') AS "File Description",
-    fd.file_type AS "File Type" ,
-        CASE     
-    WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-        END
-    WHEN fd.file_size &gt;= 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
-        END
-    WHEN fd.file_size &gt;= 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
-            ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
-        END
-    ELSE 
-        CASE 
-            WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
-            ELSE ROUND(fd.file_size, 2) || ' Bytes'
-        END
-END AS "File Size",
-fd.file_access AS "File Access", std.dbgap_accession AS "Study ID", fd.participantid AS "Participant ID", null as "Sample ID"
-FROM 
-    df_study std
- LEFT JOIN  
-    file_data fd ON std.id = fd.studyid
-WHERE 
-    std.dbgap_accession = 'phs000463'</t>
   </si>
   <si>
     <t>WITH Study AS (
@@ -228,101 +187,265 @@
     <t>TC02_CCDI_phs000463_DiagAnatSite-C42.0Blood_FirsEvent-Death_WebData.xlsx</t>
   </si>
   <si>
-    <t>SELECT
-    COUNT(DISTINCT std.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT prt.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT cmf.id)) AS "Files"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-Left JOIN 
-    df_diagnosis diag ON prt.id = diag."participant.id"  
-LEFT JOIN
-    df_survival srv ON prt.id = srv."participant.id"   
-LEFT JOIN 
-    df_clinical_measure_file cmf ON std.id = cmf."study.id"
-WHERE 
-    std.dbgap_accession = 'phs000463' AND diag.anatomic_site = 'C42.0 : Blood' AND srv.first_event ='Death' ;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    smp.anatomic_site AS "Sample Anatomic Site",
-    COALESCE(
-        CASE 
-            WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' 
-            ELSE smp.participant_age_at_collection 
-        END, 
-        0
-    ) AS "Age at Sample Collection (days)",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
-    dgn.diagnosis AS "Sample Diagnosis"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON smp.id = dgn."sample.id"
-WHERE 
-    std.dbgap_accession = 'phs000463' 
-   AND diag.anatomic_site = 'C42.0 : Blood' AND srv.first_event ='Death'
-    AND smp.sample_id IS NOT NULL
-ORDER BY 
-    smp.sample_id ASC;</t>
-  </si>
-  <si>
-    <t>with diagnosis1 as (
-select dgn."participant.id", group_concat(dgn.age_at_diagnosis,';') as age, group_concat(dgn.diagnosis,';') as diag,group_concat(dgn.anatomic_site,';') as ant_site from df_diagnosis dgn where dgn."participant.id" is not null group by dgn."participant.id" ),
-diagnosis2 as (select "participant.id",  group_concat(diagnosis,';') as diag from (select distinct "participant.id", diagnosis from df_diagnosis  where "participant.id" is not null )  group by "participant.id" ),
-diagnosis3 as (select "participant.id",  group_concat(anatomic_site,';') as ant_site from (select distinct "participant.id", anatomic_site from df_diagnosis where "participant.id" is not null ) group by "participant.id" ) 
+    <t>WITH Study AS (
+  SELECT
+    std.id              AS study_row_id,
+    std.dbgap_accession AS study_id
+  FROM df_study std
+  WHERE std.dbgap_accession = 'phs000463'
+  LIMIT 1
+),
+EligibleParticipants AS (
+  SELECT prt.id AS participant_id
+  FROM df_participant prt
+  JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  JOIN Study s            ON cg."study.id" = s.study_row_id
+  WHERE EXISTS (
+          SELECT 1
+          FROM df_diagnosis d
+          WHERE d."participant.id" = prt.id
+            AND d.anatomic_site = 'C42.0 : Blood'
+        )
+    AND EXISTS (
+          SELECT 1
+          FROM df_survival srv
+          WHERE srv."participant.id" = prt.id
+            AND srv.first_event = 'Death'
+        )
+),
+diagnosis_summary AS (
+  SELECT
+    d."participant.id"                                AS participant_id,
+    GROUP_CONCAT(DISTINCT d.age_at_diagnosis)         AS age_at_diagnosis,
+    GROUP_CONCAT(DISTINCT d.diagnosis)                AS diagnosis,
+    GROUP_CONCAT(DISTINCT d.anatomic_site)            AS anatomic_site,
+    GROUP_CONCAT(DISTINCT d.diagnosis_category)       AS diagnosis_category
+  FROM df_diagnosis d
+  JOIN EligibleParticipants ep ON ep.participant_id = d."participant.id"
+  GROUP BY d."participant.id"
+),
+survival_summary AS (
+  SELECT
+    s."participant.id"                                AS participant_id,
+    GROUP_CONCAT(DISTINCT s.last_known_survival_status) AS last_known_survival_status
+  FROM df_survival s
+  JOIN EligibleParticipants ep ON ep.participant_id = s."participant.id"
+  GROUP BY s."participant.id"
+)
+SELECT
+  prt.participant_id                           AS "Participant ID",
+  s.study_id                                   AS "Study ID",
+  COALESCE(prt.sex_at_birth, '')               AS "Sex",
+  COALESCE(prt.race, '')                       AS "Race",
+  COALESCE(dsum.diagnosis, '')                 AS "Diagnosis",
+  COALESCE(dsum.anatomic_site, '')             AS "Diagnosis Anatomic Site",
+  COALESCE(dsum.diagnosis_category, '')        AS "Diagnosis_Category",
+  COALESCE(
+    CASE WHEN dsum.age_at_diagnosis = '-999' THEN 'Not Reported' ELSE dsum.age_at_diagnosis END,
+    ''
+  )                                            AS "Age at Diagnosis (days)",
+  NULL                                         AS "Treatment Type",
+  COALESCE(srv.last_known_survival_status, '') AS "Last Known Survival Status"
+FROM EligibleParticipants ep
+JOIN df_participant prt ON prt.id = ep.participant_id
+JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+JOIN Study s ON cg."study.id" = s.study_row_id
+LEFT JOIN diagnosis_summary dsum ON dsum.participant_id = prt.id
+LEFT JOIN survival_summary  srv  ON srv.participant_id  = prt.id
+ORDER BY prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH Study AS (
+  SELECT
+    std.id              AS study_row_id,
+    std.dbgap_accession AS study_id
+  FROM df_study std
+  WHERE std.dbgap_accession = 'phs000463'
+  LIMIT 1
+),
+EligibleParticipants AS (
+  SELECT prt.id AS participant_row_id, prt.participant_id
+  FROM df_participant prt
+  JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  JOIN Study s             ON cg."study.id" = s.study_row_id
+  WHERE EXISTS (
+          SELECT 1
+          FROM df_diagnosis d
+          WHERE d."participant.id" = prt.id
+            AND d.anatomic_site = 'C42.0 : Blood'
+        )
+    AND EXISTS (
+          SELECT 1
+          FROM df_survival srv
+          WHERE srv."participant.id" = prt.id
+            AND srv.first_event = 'Death'
+        )
+),
+FilesCTE AS (
+  SELECT COUNT(DISTINCT cmf.id) AS file_count
+  FROM df_clinical_measure_file cmf
+  JOIN Study s ON cmf."study.id" = s.study_row_id
+)
+SELECT
+  COUNT(DISTINCT s.study_id)        AS "Studies",
+  COUNT(DISTINCT ep.participant_id) AS "Participants",
+  CAST(0 AS INTEGER)                AS "Samples",
+  (SELECT file_count FROM FilesCTE) AS "Files"
+FROM Study s
+LEFT JOIN EligibleParticipants ep ON 1=1;</t>
+  </si>
+  <si>
+    <t>WITH Study AS (
+  SELECT std.id AS study_row_id, std.dbgap_accession AS study_id
+  FROM df_study std
+  WHERE std.dbgap_accession = 'phs000463'
+  LIMIT 1
+),
+EligibleParticipants AS (
+  SELECT prt.id AS participant_row_id, prt.participant_id
+  FROM df_participant prt
+  JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  JOIN Study s             ON cg."study.id" = s.study_row_id
+  WHERE EXISTS (
+          SELECT 1
+          FROM df_diagnosis d
+          WHERE d."participant.id" = prt.id
+            AND d.anatomic_site = 'C42.0 : Blood'
+        )
+    AND EXISTS (
+          SELECT 1
+          FROM df_survival srv
+          WHERE srv."participant.id" = prt.id
+            AND srv.first_event = 'Death'
+        )
+),
+-- sample-level diagnosis (if any)
+SampleDiag AS (
+  SELECT d."sample.id" AS sample_row_id,
+         MAX(d.diagnosis)          AS diagnosis,
+         MAX(d.diagnosis_category) AS diagnosis_category
+  FROM df_diagnosis d
+  WHERE d."sample.id" IS NOT NULL
+  GROUP BY d."sample.id"
+)
 SELECT DISTINCT
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    COALESCE(prt.sex_at_birth, '') AS "Sex",
-    COALESCE(prt.race, '') AS "Race",
-	dgn2.diag AS "Diagnosis",
-	dgn3.ant_site AS "Diagnosis Anatomic Site",
-	   COALESCE(CASE WHEN dgn1.age = '-999' THEN 'Not Reported' ELSE dgn1.age END, "") AS "Age at Diagnosis (days)",
-	null AS "Treatment Type",
-	srv.last_known_survival_status AS "Last Known Survival Status"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    diagnosis1 dgn1 ON prt.id = dgn1."participant.id" 
-LEFT JOIN 
-    diagnosis2 dgn2 ON prt.id = dgn2."participant.id"
-LEFT JOIN 
-    diagnosis3 dgn3 ON prt.id = dgn3."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-WHERE 
-    std.dbgap_accession = 'phs000463' 
-    AND dgn.anatomic_site = 'C42.0 : Blood' 
-    AND srv.first_event ='Death'
-ORDER BY 
-    prt.participant_id ASC limit 100;</t>
+  COALESCE(smp.sample_id, smp.id)                              AS "Sample ID",
+  ep.participant_id                                            AS "Participant ID",
+  (SELECT study_id FROM Study)                                  AS "Study ID",
+  COALESCE(smp.anatomic_site, '')                              AS "Sample Anatomic Site",
+  COALESCE(
+    CASE
+      WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported'
+      ELSE CAST(smp.participant_age_at_collection AS TEXT)
+    END,
+    '0'
+  )                                                            AS "Age at Sample Collection (days)",
+  COALESCE(smp.sample_tumor_status, '')                        AS "Sample Tumor Status",
+  COALESCE(smp.tumor_classification, '')                       AS "Sample Tumor Classification",
+  sd.diagnosis                                                 AS "Sample Diagnosis",
+  COALESCE(sd.diagnosis_category, '')                          AS "Diagnosis_Category"
+FROM df_sample smp
+JOIN EligibleParticipants ep ON ep.participant_row_id = smp."participant.id"
+LEFT JOIN SampleDiag sd       ON sd.sample_row_id = smp.id
+WHERE smp.id IS NOT NULL
+ORDER BY COALESCE(smp.sample_id, smp.id) ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>WITH Study AS (
+  SELECT std.id AS study_row_id, std.dbgap_accession AS study_id
+  FROM df_study std
+  WHERE std.dbgap_accession = 'phs000463'
+  LIMIT 1
+),
+EligibleParticipants AS (
+  SELECT prt.id AS participant_row_id, prt.participant_id
+  FROM df_participant prt
+  JOIN df_consent_group cg ON prt."consent_group.id" = cg.id
+  JOIN Study s ON cg."study.id" = s.study_row_id
+  WHERE EXISTS (
+          SELECT 1
+          FROM df_diagnosis d
+          WHERE d."participant.id" = prt.id
+            AND d.anatomic_site = 'C42.0 : Blood'
+        )
+    AND EXISTS (
+          SELECT 1
+          FROM df_survival srv
+          WHERE srv."participant.id" = prt.id
+            AND srv.first_event = 'Death'
+        )
+),
+file_data AS (
+  SELECT
+    cmf.file_name,
+    REPLACE(COALESCE(cmf.data_category, ''), ';', ', ') AS data_category,
+    COALESCE(cmf.file_description, '') AS file_description,
+    cmf.file_type,
+    cmf.file_access,
+    cmf.file_size,
+    cmf."study.id" AS study_row_id,
+    cmf."participant.id" AS participant_row_id
+  FROM df_clinical_measure_file cmf
+)
+SELECT DISTINCT
+  fd.file_name AS "File Name",
+  fd.data_category AS "Data Category",
+  fd.file_description AS "File Description",
+  fd.file_type AS "File Type",
+  CASE
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 * 1024 * 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
+        ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
+      END
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 * 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
+        ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
+      END
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
+        ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
+      END
+    ELSE
+      CASE
+        WHEN ROUND(COALESCE(fd.file_size, 0), 2) = CAST(ROUND(COALESCE(fd.file_size, 0), 0) AS INT)
+        THEN CAST(CAST(ROUND(COALESCE(fd.file_size, 0), 0) AS INT) AS TEXT) || ' Bytes'
+        ELSE ROUND(COALESCE(fd.file_size, 0), 2) || ' Bytes'
+      END
+  END AS "File Size",
+  fd.file_access AS "File Access",
+  (SELECT study_id FROM Study) AS "Study ID",
+  COALESCE(ep.participant_id, '') AS "Participant ID",
+  '' AS "Sample ID"
+FROM file_data fd
+JOIN Study s ON fd.study_row_id = s.study_row_id
+LEFT JOIN EligibleParticipants ep ON ep.participant_row_id = fd.participant_row_id
+WHERE (fd.participant_row_id IS NULL OR ep.participant_row_id IS NOT NULL)
+ORDER BY fd.file_name
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -382,14 +505,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -715,19 +841,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="47.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.83203125" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" customWidth="1"/>
     <col min="5" max="5" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -744,58 +870,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="355.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="355" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>